<commit_message>
add sbp change by 10
</commit_message>
<xml_diff>
--- a/ref/Mega Data Collection Sheet.xlsx
+++ b/ref/Mega Data Collection Sheet.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\r61-r33_vccc_kumc\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F12C53-5FC7-4F02-85B0-4DA26A6359B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01F67DB-CD8B-48B3-962D-8DE827420DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mega data sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="193">
   <si>
     <t>Patient ID</t>
   </si>
@@ -662,144 +661,12 @@
   <si>
     <t>Urine Acid</t>
   </si>
-  <si>
-    <t>ANE</t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t>ARTH</t>
-  </si>
-  <si>
-    <t>AFIB</t>
-  </si>
-  <si>
-    <t>BLID</t>
-  </si>
-  <si>
-    <t>CANC</t>
-  </si>
-  <si>
-    <t>CKD</t>
-  </si>
-  <si>
-    <t>CP</t>
-  </si>
-  <si>
-    <t>CHF</t>
-  </si>
-  <si>
-    <t>CAD</t>
-  </si>
-  <si>
-    <t>DEM</t>
-  </si>
-  <si>
-    <t>DEP</t>
-  </si>
-  <si>
-    <t>DIA</t>
-  </si>
-  <si>
-    <t>DIZ</t>
-  </si>
-  <si>
-    <t>DYS</t>
-  </si>
-  <si>
-    <t>FALL</t>
-  </si>
-  <si>
-    <t>FRA</t>
-  </si>
-  <si>
-    <t>HEAR</t>
-  </si>
-  <si>
-    <t>HYPTN</t>
-  </si>
-  <si>
-    <t>SYNCO</t>
-  </si>
-  <si>
-    <t>LEUK</t>
-  </si>
-  <si>
-    <t>MLD</t>
-  </si>
-  <si>
-    <t>MSLD</t>
-  </si>
-  <si>
-    <t>MEL</t>
-  </si>
-  <si>
-    <t>MI</t>
-  </si>
-  <si>
-    <t>OST</t>
-  </si>
-  <si>
-    <t>PD</t>
-  </si>
-  <si>
-    <t>PUD</t>
-  </si>
-  <si>
-    <t>PVD</t>
-  </si>
-  <si>
-    <t>PULM</t>
-  </si>
-  <si>
-    <t>SU</t>
-  </si>
-  <si>
-    <t>STROKE</t>
-  </si>
-  <si>
-    <t>TD</t>
-  </si>
-  <si>
-    <t>UI</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>VALV</t>
-  </si>
-  <si>
-    <t>WTLOS</t>
-  </si>
-  <si>
-    <t>CTD</t>
-  </si>
-  <si>
-    <t>DKD</t>
-  </si>
-  <si>
-    <t>TIN</t>
-  </si>
-  <si>
-    <t>URO</t>
-  </si>
-  <si>
-    <t>,0)</t>
-  </si>
-  <si>
-    <t>coalesce(b.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> as </t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -842,11 +709,6 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -893,7 +755,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -948,9 +810,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1234,7 +1093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CT9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="Q6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -2381,1056 +2240,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599B471E-F994-4B6E-86BD-4999B52CE97B}">
-  <dimension ref="A1:H43"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="8" max="8" width="33.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="21"/>
-      <c r="B1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F1" t="s">
-        <v>193</v>
-      </c>
-      <c r="H1" t="str">
-        <f>_xlfn.CONCAT(B1,C1,D1)</f>
-        <v>coalesce(b.ANE,0)</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E2" t="s">
-        <v>236</v>
-      </c>
-      <c r="F2" t="s">
-        <v>195</v>
-      </c>
-      <c r="H2" t="str">
-        <f>_xlfn.CONCAT(B2,C2,D2)</f>
-        <v>coalesce(b.ARTH,0)</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E3" t="s">
-        <v>236</v>
-      </c>
-      <c r="F3" t="s">
-        <v>196</v>
-      </c>
-      <c r="H3" t="str">
-        <f>_xlfn.CONCAT(B3,C3,D3)</f>
-        <v>coalesce(b.AFIB,0)</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B4" t="s">
-        <v>235</v>
-      </c>
-      <c r="C4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" t="s">
-        <v>234</v>
-      </c>
-      <c r="E4" t="s">
-        <v>236</v>
-      </c>
-      <c r="F4" t="s">
-        <v>197</v>
-      </c>
-      <c r="H4" t="str">
-        <f>_xlfn.CONCAT(B4,C4,D4)</f>
-        <v>coalesce(b.BLID,0)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B5" t="s">
-        <v>235</v>
-      </c>
-      <c r="C5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D5" t="s">
-        <v>234</v>
-      </c>
-      <c r="E5" t="s">
-        <v>236</v>
-      </c>
-      <c r="F5" t="s">
-        <v>198</v>
-      </c>
-      <c r="H5" t="str">
-        <f>_xlfn.CONCAT(B5,C5,D5)</f>
-        <v>coalesce(b.CANC,0)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B6" t="s">
-        <v>235</v>
-      </c>
-      <c r="C6" t="s">
-        <v>199</v>
-      </c>
-      <c r="D6" t="s">
-        <v>234</v>
-      </c>
-      <c r="E6" t="s">
-        <v>236</v>
-      </c>
-      <c r="F6" t="s">
-        <v>199</v>
-      </c>
-      <c r="H6" t="str">
-        <f>_xlfn.CONCAT(B6,C6,D6)</f>
-        <v>coalesce(b.CKD,0)</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B7" t="s">
-        <v>235</v>
-      </c>
-      <c r="C7" t="s">
-        <v>200</v>
-      </c>
-      <c r="D7" t="s">
-        <v>234</v>
-      </c>
-      <c r="E7" t="s">
-        <v>236</v>
-      </c>
-      <c r="F7" t="s">
-        <v>200</v>
-      </c>
-      <c r="H7" t="str">
-        <f>_xlfn.CONCAT(B7,C7,D7)</f>
-        <v>coalesce(b.CP,0)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B8" t="s">
-        <v>235</v>
-      </c>
-      <c r="C8" t="s">
-        <v>201</v>
-      </c>
-      <c r="D8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E8" t="s">
-        <v>236</v>
-      </c>
-      <c r="F8" t="s">
-        <v>201</v>
-      </c>
-      <c r="H8" t="str">
-        <f>_xlfn.CONCAT(B8,C8,D8)</f>
-        <v>coalesce(b.CHF,0)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B9" t="s">
-        <v>235</v>
-      </c>
-      <c r="C9" t="s">
-        <v>202</v>
-      </c>
-      <c r="D9" t="s">
-        <v>234</v>
-      </c>
-      <c r="E9" t="s">
-        <v>236</v>
-      </c>
-      <c r="F9" t="s">
-        <v>202</v>
-      </c>
-      <c r="H9" t="str">
-        <f>_xlfn.CONCAT(B9,C9,D9)</f>
-        <v>coalesce(b.CAD,0)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B10" t="s">
-        <v>235</v>
-      </c>
-      <c r="C10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D10" t="s">
-        <v>234</v>
-      </c>
-      <c r="E10" t="s">
-        <v>236</v>
-      </c>
-      <c r="F10" t="s">
-        <v>203</v>
-      </c>
-      <c r="H10" t="str">
-        <f>_xlfn.CONCAT(B10,C10,D10)</f>
-        <v>coalesce(b.DEM,0)</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B11" t="s">
-        <v>235</v>
-      </c>
-      <c r="C11" t="s">
-        <v>204</v>
-      </c>
-      <c r="D11" t="s">
-        <v>234</v>
-      </c>
-      <c r="E11" t="s">
-        <v>236</v>
-      </c>
-      <c r="F11" t="s">
-        <v>204</v>
-      </c>
-      <c r="H11" t="str">
-        <f>_xlfn.CONCAT(B11,C11,D11)</f>
-        <v>coalesce(b.DEP,0)</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B12" t="s">
-        <v>235</v>
-      </c>
-      <c r="C12" t="s">
-        <v>205</v>
-      </c>
-      <c r="D12" t="s">
-        <v>234</v>
-      </c>
-      <c r="E12" t="s">
-        <v>236</v>
-      </c>
-      <c r="F12" t="s">
-        <v>205</v>
-      </c>
-      <c r="H12" t="str">
-        <f>_xlfn.CONCAT(B12,C12,D12)</f>
-        <v>coalesce(b.DIA,0)</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B13" t="s">
-        <v>235</v>
-      </c>
-      <c r="C13" t="s">
-        <v>206</v>
-      </c>
-      <c r="D13" t="s">
-        <v>234</v>
-      </c>
-      <c r="E13" t="s">
-        <v>236</v>
-      </c>
-      <c r="F13" t="s">
-        <v>206</v>
-      </c>
-      <c r="H13" t="str">
-        <f>_xlfn.CONCAT(B13,C13,D13)</f>
-        <v>coalesce(b.DIZ,0)</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B14" t="s">
-        <v>235</v>
-      </c>
-      <c r="C14" t="s">
-        <v>207</v>
-      </c>
-      <c r="D14" t="s">
-        <v>234</v>
-      </c>
-      <c r="E14" t="s">
-        <v>236</v>
-      </c>
-      <c r="F14" t="s">
-        <v>207</v>
-      </c>
-      <c r="H14" t="str">
-        <f>_xlfn.CONCAT(B14,C14,D14)</f>
-        <v>coalesce(b.DYS,0)</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B15" t="s">
-        <v>235</v>
-      </c>
-      <c r="C15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D15" t="s">
-        <v>234</v>
-      </c>
-      <c r="E15" t="s">
-        <v>236</v>
-      </c>
-      <c r="F15" t="s">
-        <v>208</v>
-      </c>
-      <c r="H15" t="str">
-        <f>_xlfn.CONCAT(B15,C15,D15)</f>
-        <v>coalesce(b.FALL,0)</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B16" t="s">
-        <v>235</v>
-      </c>
-      <c r="C16" t="s">
-        <v>209</v>
-      </c>
-      <c r="D16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E16" t="s">
-        <v>236</v>
-      </c>
-      <c r="F16" t="s">
-        <v>209</v>
-      </c>
-      <c r="H16" t="str">
-        <f>_xlfn.CONCAT(B16,C16,D16)</f>
-        <v>coalesce(b.FRA,0)</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B17" t="s">
-        <v>235</v>
-      </c>
-      <c r="C17" t="s">
-        <v>210</v>
-      </c>
-      <c r="D17" t="s">
-        <v>234</v>
-      </c>
-      <c r="E17" t="s">
-        <v>236</v>
-      </c>
-      <c r="F17" t="s">
-        <v>210</v>
-      </c>
-      <c r="H17" t="str">
-        <f>_xlfn.CONCAT(B17,C17,D17)</f>
-        <v>coalesce(b.HEAR,0)</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B18" t="s">
-        <v>235</v>
-      </c>
-      <c r="C18" t="s">
-        <v>211</v>
-      </c>
-      <c r="D18" t="s">
-        <v>234</v>
-      </c>
-      <c r="E18" t="s">
-        <v>236</v>
-      </c>
-      <c r="F18" t="s">
-        <v>211</v>
-      </c>
-      <c r="H18" t="str">
-        <f>_xlfn.CONCAT(B18,C18,D18)</f>
-        <v>coalesce(b.HYPTN,0)</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B19" t="s">
-        <v>235</v>
-      </c>
-      <c r="C19" t="s">
-        <v>212</v>
-      </c>
-      <c r="D19" t="s">
-        <v>234</v>
-      </c>
-      <c r="E19" t="s">
-        <v>236</v>
-      </c>
-      <c r="F19" t="s">
-        <v>212</v>
-      </c>
-      <c r="H19" t="str">
-        <f>_xlfn.CONCAT(B19,C19,D19)</f>
-        <v>coalesce(b.SYNCO,0)</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B20" t="s">
-        <v>235</v>
-      </c>
-      <c r="C20" t="s">
-        <v>213</v>
-      </c>
-      <c r="D20" t="s">
-        <v>234</v>
-      </c>
-      <c r="E20" t="s">
-        <v>236</v>
-      </c>
-      <c r="F20" t="s">
-        <v>213</v>
-      </c>
-      <c r="H20" t="str">
-        <f>_xlfn.CONCAT(B20,C20,D20)</f>
-        <v>coalesce(b.LEUK,0)</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B21" t="s">
-        <v>235</v>
-      </c>
-      <c r="C21" t="s">
-        <v>214</v>
-      </c>
-      <c r="D21" t="s">
-        <v>234</v>
-      </c>
-      <c r="E21" t="s">
-        <v>236</v>
-      </c>
-      <c r="F21" t="s">
-        <v>214</v>
-      </c>
-      <c r="H21" t="str">
-        <f>_xlfn.CONCAT(B21,C21,D21)</f>
-        <v>coalesce(b.MLD,0)</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B22" t="s">
-        <v>235</v>
-      </c>
-      <c r="C22" t="s">
-        <v>215</v>
-      </c>
-      <c r="D22" t="s">
-        <v>234</v>
-      </c>
-      <c r="E22" t="s">
-        <v>236</v>
-      </c>
-      <c r="F22" t="s">
-        <v>215</v>
-      </c>
-      <c r="H22" t="str">
-        <f>_xlfn.CONCAT(B22,C22,D22)</f>
-        <v>coalesce(b.MSLD,0)</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B23" t="s">
-        <v>235</v>
-      </c>
-      <c r="C23" t="s">
-        <v>216</v>
-      </c>
-      <c r="D23" t="s">
-        <v>234</v>
-      </c>
-      <c r="E23" t="s">
-        <v>236</v>
-      </c>
-      <c r="F23" t="s">
-        <v>216</v>
-      </c>
-      <c r="H23" t="str">
-        <f>_xlfn.CONCAT(B23,C23,D23)</f>
-        <v>coalesce(b.MEL,0)</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B24" t="s">
-        <v>235</v>
-      </c>
-      <c r="C24" t="s">
-        <v>217</v>
-      </c>
-      <c r="D24" t="s">
-        <v>234</v>
-      </c>
-      <c r="E24" t="s">
-        <v>236</v>
-      </c>
-      <c r="F24" t="s">
-        <v>217</v>
-      </c>
-      <c r="H24" t="str">
-        <f>_xlfn.CONCAT(B24,C24,D24)</f>
-        <v>coalesce(b.MI,0)</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B25" t="s">
-        <v>235</v>
-      </c>
-      <c r="C25" t="s">
-        <v>218</v>
-      </c>
-      <c r="D25" t="s">
-        <v>234</v>
-      </c>
-      <c r="E25" t="s">
-        <v>236</v>
-      </c>
-      <c r="F25" t="s">
-        <v>218</v>
-      </c>
-      <c r="H25" t="str">
-        <f>_xlfn.CONCAT(B25,C25,D25)</f>
-        <v>coalesce(b.OST,0)</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B26" t="s">
-        <v>235</v>
-      </c>
-      <c r="C26" t="s">
-        <v>219</v>
-      </c>
-      <c r="D26" t="s">
-        <v>234</v>
-      </c>
-      <c r="E26" t="s">
-        <v>236</v>
-      </c>
-      <c r="F26" t="s">
-        <v>219</v>
-      </c>
-      <c r="H26" t="str">
-        <f>_xlfn.CONCAT(B26,C26,D26)</f>
-        <v>coalesce(b.PD,0)</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B27" t="s">
-        <v>235</v>
-      </c>
-      <c r="C27" t="s">
-        <v>220</v>
-      </c>
-      <c r="D27" t="s">
-        <v>234</v>
-      </c>
-      <c r="E27" t="s">
-        <v>236</v>
-      </c>
-      <c r="F27" t="s">
-        <v>220</v>
-      </c>
-      <c r="H27" t="str">
-        <f>_xlfn.CONCAT(B27,C27,D27)</f>
-        <v>coalesce(b.PUD,0)</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B28" t="s">
-        <v>235</v>
-      </c>
-      <c r="C28" t="s">
-        <v>221</v>
-      </c>
-      <c r="D28" t="s">
-        <v>234</v>
-      </c>
-      <c r="E28" t="s">
-        <v>236</v>
-      </c>
-      <c r="F28" t="s">
-        <v>221</v>
-      </c>
-      <c r="H28" t="str">
-        <f>_xlfn.CONCAT(B28,C28,D28)</f>
-        <v>coalesce(b.PVD,0)</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B29" t="s">
-        <v>235</v>
-      </c>
-      <c r="C29" t="s">
-        <v>222</v>
-      </c>
-      <c r="D29" t="s">
-        <v>234</v>
-      </c>
-      <c r="E29" t="s">
-        <v>236</v>
-      </c>
-      <c r="F29" t="s">
-        <v>222</v>
-      </c>
-      <c r="H29" t="str">
-        <f>_xlfn.CONCAT(B29,C29,D29)</f>
-        <v>coalesce(b.PULM,0)</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B30" t="s">
-        <v>235</v>
-      </c>
-      <c r="C30" t="s">
-        <v>223</v>
-      </c>
-      <c r="D30" t="s">
-        <v>234</v>
-      </c>
-      <c r="E30" t="s">
-        <v>236</v>
-      </c>
-      <c r="F30" t="s">
-        <v>223</v>
-      </c>
-      <c r="H30" t="str">
-        <f>_xlfn.CONCAT(B30,C30,D30)</f>
-        <v>coalesce(b.SU,0)</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B31" t="s">
-        <v>235</v>
-      </c>
-      <c r="C31" t="s">
-        <v>224</v>
-      </c>
-      <c r="D31" t="s">
-        <v>234</v>
-      </c>
-      <c r="E31" t="s">
-        <v>236</v>
-      </c>
-      <c r="F31" t="s">
-        <v>224</v>
-      </c>
-      <c r="H31" t="str">
-        <f>_xlfn.CONCAT(B31,C31,D31)</f>
-        <v>coalesce(b.STROKE,0)</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B32" t="s">
-        <v>235</v>
-      </c>
-      <c r="C32" t="s">
-        <v>225</v>
-      </c>
-      <c r="D32" t="s">
-        <v>234</v>
-      </c>
-      <c r="E32" t="s">
-        <v>236</v>
-      </c>
-      <c r="F32" t="s">
-        <v>225</v>
-      </c>
-      <c r="H32" t="str">
-        <f>_xlfn.CONCAT(B32,C32,D32)</f>
-        <v>coalesce(b.TD,0)</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B33" t="s">
-        <v>235</v>
-      </c>
-      <c r="C33" t="s">
-        <v>226</v>
-      </c>
-      <c r="D33" t="s">
-        <v>234</v>
-      </c>
-      <c r="E33" t="s">
-        <v>236</v>
-      </c>
-      <c r="F33" t="s">
-        <v>226</v>
-      </c>
-      <c r="H33" t="str">
-        <f>_xlfn.CONCAT(B33,C33,D33)</f>
-        <v>coalesce(b.UI,0)</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B34" t="s">
-        <v>235</v>
-      </c>
-      <c r="C34" t="s">
-        <v>227</v>
-      </c>
-      <c r="D34" t="s">
-        <v>234</v>
-      </c>
-      <c r="E34" t="s">
-        <v>236</v>
-      </c>
-      <c r="F34" t="s">
-        <v>227</v>
-      </c>
-      <c r="H34" t="str">
-        <f>_xlfn.CONCAT(B34,C34,D34)</f>
-        <v>coalesce(b.USD,0)</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B35" t="s">
-        <v>235</v>
-      </c>
-      <c r="C35" t="s">
-        <v>228</v>
-      </c>
-      <c r="D35" t="s">
-        <v>234</v>
-      </c>
-      <c r="E35" t="s">
-        <v>236</v>
-      </c>
-      <c r="F35" t="s">
-        <v>228</v>
-      </c>
-      <c r="H35" t="str">
-        <f>_xlfn.CONCAT(B35,C35,D35)</f>
-        <v>coalesce(b.VALV,0)</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B36" t="s">
-        <v>235</v>
-      </c>
-      <c r="C36" t="s">
-        <v>229</v>
-      </c>
-      <c r="D36" t="s">
-        <v>234</v>
-      </c>
-      <c r="E36" t="s">
-        <v>236</v>
-      </c>
-      <c r="F36" t="s">
-        <v>229</v>
-      </c>
-      <c r="H36" t="str">
-        <f>_xlfn.CONCAT(B36,C36,D36)</f>
-        <v>coalesce(b.WTLOS,0)</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B37" t="s">
-        <v>235</v>
-      </c>
-      <c r="C37" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" t="s">
-        <v>234</v>
-      </c>
-      <c r="E37" t="s">
-        <v>236</v>
-      </c>
-      <c r="F37" t="s">
-        <v>54</v>
-      </c>
-      <c r="H37" t="str">
-        <f>_xlfn.CONCAT(B37,C37,D37)</f>
-        <v>coalesce(b.AIDS,0)</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B38" t="s">
-        <v>235</v>
-      </c>
-      <c r="C38" t="s">
-        <v>230</v>
-      </c>
-      <c r="D38" t="s">
-        <v>234</v>
-      </c>
-      <c r="E38" t="s">
-        <v>236</v>
-      </c>
-      <c r="F38" t="s">
-        <v>230</v>
-      </c>
-      <c r="H38" t="str">
-        <f>_xlfn.CONCAT(B38,C38,D38)</f>
-        <v>coalesce(b.CTD,0)</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B39" t="s">
-        <v>235</v>
-      </c>
-      <c r="C39" t="s">
-        <v>231</v>
-      </c>
-      <c r="D39" t="s">
-        <v>234</v>
-      </c>
-      <c r="E39" t="s">
-        <v>236</v>
-      </c>
-      <c r="F39" t="s">
-        <v>231</v>
-      </c>
-      <c r="H39" t="str">
-        <f>_xlfn.CONCAT(B39,C39,D39)</f>
-        <v>coalesce(b.DKD,0)</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B40" t="s">
-        <v>235</v>
-      </c>
-      <c r="C40" t="s">
-        <v>121</v>
-      </c>
-      <c r="D40" t="s">
-        <v>234</v>
-      </c>
-      <c r="E40" t="s">
-        <v>236</v>
-      </c>
-      <c r="F40" t="s">
-        <v>121</v>
-      </c>
-      <c r="H40" t="str">
-        <f>_xlfn.CONCAT(B40,C40,D40)</f>
-        <v>coalesce(b.ADPKD,0)</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B41" t="s">
-        <v>235</v>
-      </c>
-      <c r="C41" t="s">
-        <v>129</v>
-      </c>
-      <c r="D41" t="s">
-        <v>234</v>
-      </c>
-      <c r="E41" t="s">
-        <v>236</v>
-      </c>
-      <c r="F41" t="s">
-        <v>129</v>
-      </c>
-      <c r="H41" t="str">
-        <f>_xlfn.CONCAT(B41,C41,D41)</f>
-        <v>coalesce(b.GN,0)</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B42" t="s">
-        <v>235</v>
-      </c>
-      <c r="C42" t="s">
-        <v>232</v>
-      </c>
-      <c r="D42" t="s">
-        <v>234</v>
-      </c>
-      <c r="E42" t="s">
-        <v>236</v>
-      </c>
-      <c r="F42" t="s">
-        <v>232</v>
-      </c>
-      <c r="H42" t="str">
-        <f>_xlfn.CONCAT(B42,C42,D42)</f>
-        <v>coalesce(b.TIN,0)</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B43" t="s">
-        <v>235</v>
-      </c>
-      <c r="C43" t="s">
-        <v>233</v>
-      </c>
-      <c r="D43" t="s">
-        <v>234</v>
-      </c>
-      <c r="E43" t="s">
-        <v>236</v>
-      </c>
-      <c r="F43" t="s">
-        <v>233</v>
-      </c>
-      <c r="H43" t="str">
-        <f>_xlfn.CONCAT(B43,C43,D43)</f>
-        <v>coalesce(b.URO,0)</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="70e68cd6-7252-44ce-bf81-24cb873d0ea8" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bd33661-7264-4633-9226-fba6aeef08ea">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Comment xmlns="9bd33661-7264-4633-9226-fba6aeef08ea" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100066C90EDBA55B24994D27E40D9B366FA" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0abdc5e5dcc78fc5633c117b6ca51f6f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="70e68cd6-7252-44ce-bf81-24cb873d0ea8" xmlns:ns3="9bd33661-7264-4633-9226-fba6aeef08ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e1a8588803c1425044082fb2e72aebb3" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3710,30 +2543,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7049147A-FDA0-4A3F-B2DE-8F662652CBA3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="70e68cd6-7252-44ce-bf81-24cb873d0ea8"/>
+    <ds:schemaRef ds:uri="9bd33661-7264-4633-9226-fba6aeef08ea"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="70e68cd6-7252-44ce-bf81-24cb873d0ea8" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bd33661-7264-4633-9226-fba6aeef08ea">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Comment xmlns="9bd33661-7264-4633-9226-fba6aeef08ea" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2924868A-51E0-4221-8368-AE9A7E1C2DCD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{730A057D-63DA-492E-AFBD-277C6BE8B76F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3751,24 +2581,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2924868A-51E0-4221-8368-AE9A7E1C2DCD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7049147A-FDA0-4A3F-B2DE-8F662652CBA3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="70e68cd6-7252-44ce-bf81-24cb873d0ea8"/>
-    <ds:schemaRef ds:uri="9bd33661-7264-4633-9226-fba6aeef08ea"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>